<commit_message>
correct saleTable singleCost not the same
</commit_message>
<xml_diff>
--- a/server/excels/manualSale.xlsx
+++ b/server/excels/manualSale.xlsx
@@ -10,7 +10,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="15">
+  <numFmts count="16">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="7" formatCode="&quot;¥&quot;#,##0.00;&quot;¥&quot;\-#,##0.00"/>
@@ -23,9 +23,10 @@
     <numFmt numFmtId="42" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="#,###,###,##0.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="176" formatCode="&quot;Yes&quot;;&quot;Yes&quot;;&quot;No&quot;"/>
+    <numFmt numFmtId="177" formatCode="&quot;True&quot;;&quot;True&quot;;&quot;False&quot;"/>
+    <numFmt numFmtId="178" formatCode="&quot;On&quot;;&quot;On&quot;;&quot;Off&quot;"/>
+    <numFmt numFmtId="179" formatCode="[$€-2]\ #,##0.00_);[Red]\([$€-2]\ #,##0.00\)"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -389,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D36"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -517,155 +518,276 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>090164</v>
+        <v>060143</v>
       </c>
       <c r="B12" t="str">
-        <v>三角电钣饭锅</v>
+        <v>苏泊尔水煲</v>
       </c>
       <c r="D12">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>090359</v>
+        <v>090150</v>
       </c>
       <c r="B13" t="str">
-        <v>半球电水煲2L</v>
+        <v>水煲</v>
       </c>
       <c r="D13">
-        <v>39</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>135233234</v>
+        <v>090163</v>
       </c>
       <c r="B14" t="str">
-        <v>闹钟</v>
+        <v>永兴3L火锅JQH-100</v>
       </c>
       <c r="D14">
-        <v>18</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>135015</v>
+        <v>090164</v>
       </c>
       <c r="B15" t="str">
-        <v>LED彩色小夜灯</v>
+        <v>三角电钣饭锅</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>6927065410459</v>
+        <v>090359</v>
       </c>
       <c r="B16" t="str">
-        <v>1021空调扇</v>
+        <v>半球电水煲2L</v>
       </c>
       <c r="D16">
-        <v>350</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>135011</v>
+        <v>135233234</v>
       </c>
       <c r="B17" t="str">
-        <v>万意款节王4#节能双灶</v>
+        <v>闹钟</v>
       </c>
       <c r="D17">
-        <v>78.4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>6927065400788</v>
+        <v>135015</v>
       </c>
       <c r="B18" t="str">
-        <v>DL0740电风扇</v>
+        <v>LED彩色小夜灯</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>6926159300034</v>
+        <v>6927065410459</v>
       </c>
       <c r="B19" t="str">
-        <v>低碳节能小夜灯</v>
+        <v>1021空调扇</v>
       </c>
       <c r="D19">
-        <v>9.9</v>
+        <v>350</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>6950610208522</v>
+        <v>135012</v>
       </c>
       <c r="B20" t="str">
-        <v>苏泊尔电水煲1702A</v>
+        <v>低碳无福射节能灯（大）</v>
       </c>
       <c r="D20">
-        <v>169</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>135012</v>
+        <v>135011</v>
       </c>
       <c r="B21" t="str">
-        <v>大夜灯</v>
+        <v>万意款节王4#节能双灶</v>
       </c>
       <c r="D21">
-        <v>12.75</v>
+        <v>78.4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>091469</v>
+        <v>6927065400788</v>
       </c>
       <c r="B22" t="str">
-        <v>1535电风扇</v>
+        <v>DL0740电风扇</v>
       </c>
       <c r="D22">
-        <v>169</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>091514</v>
+        <v>6926159300034</v>
       </c>
       <c r="B23" t="str">
-        <v>低碳无福射节能灯（大）</v>
+        <v>低碳节能小夜灯</v>
       </c>
       <c r="D23">
-        <v>12</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>091545</v>
+        <v>6950610208522</v>
       </c>
       <c r="B24" t="str">
-        <v>LED彩色小夜灯</v>
+        <v>苏泊尔电水煲1702A</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
+        <v>041184</v>
+      </c>
+      <c r="B25" t="str">
+        <v>炊大皇不沾锅</v>
+      </c>
+      <c r="D25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>060151</v>
+      </c>
+      <c r="B26" t="str">
+        <v>苏泊尔电饼档</v>
+      </c>
+      <c r="D26">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>060158</v>
+      </c>
+      <c r="B27" t="str">
+        <v>苏泊尔电饭煲</v>
+      </c>
+      <c r="D27">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>060168</v>
+      </c>
+      <c r="B28" t="str">
+        <v>苏泊尔迷你电饭煲</v>
+      </c>
+      <c r="D28">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>090149</v>
+      </c>
+      <c r="B29" t="str">
+        <v>电压力锅</v>
+      </c>
+      <c r="D29">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>090165</v>
+      </c>
+      <c r="B30" t="str">
+        <v>三角电饭锅</v>
+      </c>
+      <c r="D30">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>090166</v>
+      </c>
+      <c r="B31" t="str">
+        <v>三角电饭锅</v>
+      </c>
+      <c r="D31">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>091456</v>
+      </c>
+      <c r="B32" t="str">
+        <v>FSJ-180学生扇</v>
+      </c>
+      <c r="D32">
+        <v>57.8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>091469</v>
+      </c>
+      <c r="B33" t="str">
+        <v>1535电风扇</v>
+      </c>
+      <c r="D33">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>091514</v>
+      </c>
+      <c r="B34" t="str">
+        <v>低碳无福射节能灯（大）</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>091545</v>
+      </c>
+      <c r="B35" t="str">
+        <v>LED彩色小夜灯</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
         <v>091546</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B36" t="str">
         <v>低碳节能小夜灯</v>
       </c>
-      <c r="D25">
+      <c r="D36">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
check barCode same but the productName not the same
</commit_message>
<xml_diff>
--- a/server/excels/manualSale.xlsx
+++ b/server/excels/manualSale.xlsx
@@ -10,7 +10,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="15">
+  <numFmts count="16">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="7" formatCode="&quot;¥&quot;#,##0.00;&quot;¥&quot;\-#,##0.00"/>
@@ -23,9 +23,10 @@
     <numFmt numFmtId="42" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="#,###,###,##0.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="176" formatCode="&quot;Yes&quot;;&quot;Yes&quot;;&quot;No&quot;"/>
+    <numFmt numFmtId="177" formatCode="&quot;True&quot;;&quot;True&quot;;&quot;False&quot;"/>
+    <numFmt numFmtId="178" formatCode="&quot;On&quot;;&quot;On&quot;;&quot;Off&quot;"/>
+    <numFmt numFmtId="179" formatCode="[$€-2]\ #,##0.00_);[Red]\([$€-2]\ #,##0.00\)"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -389,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D36"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -638,166 +639,155 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>6927065400542</v>
+        <v>6926159300034</v>
       </c>
       <c r="B23" t="str">
-        <v>DS72升降遥控电风扇</v>
+        <v>低碳节能小夜灯</v>
       </c>
       <c r="D23">
-        <v>7.2</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>6926159300034</v>
+        <v>6950610208522</v>
       </c>
       <c r="B24" t="str">
-        <v>低碳节能小夜灯</v>
+        <v>苏泊尔电水煲1702A</v>
       </c>
       <c r="D24">
-        <v>9.9</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>6950610208522</v>
+        <v>041184</v>
       </c>
       <c r="B25" t="str">
-        <v>苏泊尔电水煲1702A</v>
+        <v>炊大皇不沾锅</v>
       </c>
       <c r="D25">
-        <v>169</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>041184</v>
+        <v>060151</v>
       </c>
       <c r="B26" t="str">
-        <v>炊大皇不沾锅</v>
+        <v>苏泊尔电饼档</v>
       </c>
       <c r="D26">
-        <v>188</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>060151</v>
+        <v>060158</v>
       </c>
       <c r="B27" t="str">
-        <v>苏泊尔电饼档</v>
+        <v>苏泊尔电饭煲</v>
       </c>
       <c r="D27">
-        <v>229</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>060158</v>
+        <v>060168</v>
       </c>
       <c r="B28" t="str">
-        <v>苏泊尔电饭煲</v>
+        <v>苏泊尔迷你电饭煲</v>
       </c>
       <c r="D28">
-        <v>159</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>060168</v>
+        <v>090149</v>
       </c>
       <c r="B29" t="str">
-        <v>苏泊尔迷你电饭煲</v>
+        <v>电压力锅</v>
       </c>
       <c r="D29">
-        <v>199</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>090149</v>
+        <v>090165</v>
       </c>
       <c r="B30" t="str">
-        <v>电压力锅</v>
+        <v>三角电饭锅</v>
       </c>
       <c r="D30">
-        <v>499</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>090165</v>
+        <v>090166</v>
       </c>
       <c r="B31" t="str">
         <v>三角电饭锅</v>
       </c>
       <c r="D31">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>090166</v>
+        <v>091456</v>
       </c>
       <c r="B32" t="str">
-        <v>三角电饭锅</v>
+        <v>FSJ-180学生扇</v>
       </c>
       <c r="D32">
-        <v>138</v>
+        <v>57.8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>091456</v>
+        <v>091469</v>
       </c>
       <c r="B33" t="str">
-        <v>FSJ-180学生扇</v>
+        <v>1535电风扇</v>
       </c>
       <c r="D33">
-        <v>57.8</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>091469</v>
+        <v>091514</v>
       </c>
       <c r="B34" t="str">
-        <v>1535电风扇</v>
+        <v>低碳无福射节能灯（大）</v>
       </c>
       <c r="D34">
-        <v>169</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>091514</v>
+        <v>091545</v>
       </c>
       <c r="B35" t="str">
-        <v>低碳无福射节能灯（大）</v>
+        <v>LED彩色小夜灯</v>
       </c>
       <c r="D35">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>091545</v>
+        <v>091546</v>
       </c>
       <c r="B36" t="str">
-        <v>LED彩色小夜灯</v>
+        <v>低碳节能小夜灯</v>
       </c>
       <c r="D36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>091546</v>
-      </c>
-      <c r="B37" t="str">
-        <v>低碳节能小夜灯</v>
-      </c>
-      <c r="D37">
         <v>8</v>
       </c>
     </row>

</xml_diff>